<commit_message>
feat(import) Import / export from xlsx files ok
</commit_message>
<xml_diff>
--- a/FlOpEDT/configuration/xls/empty_planif_file.xlsx
+++ b/FlOpEDT/configuration/xls/empty_planif_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="empty" sheetId="1" state="visible" r:id="rId2"/>
@@ -235,8 +235,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -824,7 +825,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="24" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -842,12 +843,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -913,34 +914,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:DG9"/>
+  <dimension ref="A1:DG687"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.56"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="8" style="0" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="29" style="0" width="2.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="34" style="0" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="55" style="0" width="2.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="60" style="0" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="81" style="0" width="2.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="86" style="0" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="111" min="107" style="0" width="2.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="997" min="112" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="998" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="111" min="8" style="0" width="4.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="998" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2541,8 +2534,8 @@
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2551,22 +2544,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="135" min="2" style="0" width="6.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="136" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,7 +2897,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -2914,27 +2906,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AV3"/>
+  <dimension ref="A1:CX3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BJ16" activeCellId="0" sqref="BJ16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AZ21" activeCellId="0" sqref="AZ21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="0" width="3.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="21" style="0" width="2.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="3.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="3.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="32" style="0" width="3.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="49" style="0" width="4.93"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="72" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="3" style="0" width="4.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="63" style="0" width="4.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="71" style="0" width="4.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2945,142 +2932,304 @@
         <v>43</v>
       </c>
       <c r="C1" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="V1" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W1" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="X1" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="D1" s="3" t="n">
+      <c r="AL1" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="E1" s="3" t="n">
+      <c r="AM1" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="F1" s="3" t="n">
+      <c r="AN1" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="G1" s="3" t="n">
+      <c r="AO1" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="H1" s="3" t="n">
+      <c r="AP1" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="AQ1" s="3" t="n">
         <v>41</v>
       </c>
-      <c r="J1" s="3" t="n">
+      <c r="AR1" s="3" t="n">
         <v>42</v>
       </c>
-      <c r="K1" s="3" t="n">
+      <c r="AS1" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="L1" s="3" t="n">
+      <c r="AT1" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="M1" s="3" t="n">
+      <c r="AU1" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="N1" s="3" t="n">
+      <c r="AV1" s="3" t="n">
         <v>46</v>
       </c>
-      <c r="O1" s="3" t="n">
+      <c r="AW1" s="3" t="n">
         <v>47</v>
       </c>
-      <c r="P1" s="3" t="n">
+      <c r="AX1" s="3" t="n">
         <v>48</v>
       </c>
-      <c r="Q1" s="3" t="n">
+      <c r="AY1" s="3" t="n">
         <v>49</v>
       </c>
-      <c r="R1" s="3" t="n">
+      <c r="AZ1" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="S1" s="3" t="n">
+      <c r="BA1" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="T1" s="3" t="n">
+      <c r="BB1" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="U1" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="V1" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="W1" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="X1" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="Y1" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="Z1" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AA1" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="AB1" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="AC1" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="AD1" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="AE1" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="AF1" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="AG1" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="AH1" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="AI1" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="AJ1" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="AK1" s="3" t="n">
-        <v>17</v>
-      </c>
-      <c r="AL1" s="3" t="n">
-        <v>18</v>
-      </c>
-      <c r="AM1" s="3" t="n">
-        <v>19</v>
-      </c>
-      <c r="AN1" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="AO1" s="3" t="n">
-        <v>21</v>
-      </c>
-      <c r="AP1" s="3" t="n">
-        <v>22</v>
-      </c>
-      <c r="AQ1" s="3" t="n">
-        <v>23</v>
-      </c>
-      <c r="AR1" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="AS1" s="3" t="n">
-        <v>25</v>
-      </c>
-      <c r="AT1" s="3" t="n">
-        <v>26</v>
-      </c>
-      <c r="AU1" s="3" t="n">
-        <v>27</v>
-      </c>
-      <c r="AV1" s="3" t="n">
-        <v>28</v>
+      <c r="BC1" s="3" t="n">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="3" t="n">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="3" t="n">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="3" t="n">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="3" t="n">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="3" t="n">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="3" t="n">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="3" t="n">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="3" t="n">
+        <v>67</v>
+      </c>
+      <c r="BR1" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="BS1" s="3" t="n">
+        <v>69</v>
+      </c>
+      <c r="BT1" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="BU1" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="BV1" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="BW1" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="BX1" s="3" t="n">
+        <v>74</v>
+      </c>
+      <c r="BY1" s="3" t="n">
+        <v>75</v>
+      </c>
+      <c r="BZ1" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="CA1" s="3" t="n">
+        <v>77</v>
+      </c>
+      <c r="CB1" s="3" t="n">
+        <v>78</v>
+      </c>
+      <c r="CC1" s="3" t="n">
+        <v>79</v>
+      </c>
+      <c r="CD1" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="CE1" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="CF1" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="CG1" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="CH1" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="CI1" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="CJ1" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="CK1" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="CL1" s="3" t="n">
+        <v>88</v>
+      </c>
+      <c r="CM1" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="CN1" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="CO1" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="CP1" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="CQ1" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="CR1" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="CS1" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="CT1" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="CU1" s="3" t="n">
+        <v>97</v>
+      </c>
+      <c r="CV1" s="3" t="n">
+        <v>98</v>
+      </c>
+      <c r="CW1" s="3" t="n">
+        <v>99</v>
+      </c>
+      <c r="CX1" s="3" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3269,6 +3418,222 @@
         <v>0</v>
       </c>
       <c r="AV2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AW2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AX2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AY2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BA2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BB2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BC2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BD2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BE2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BF2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BG2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BH2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BI2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BJ2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BK2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BL2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BM2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BN2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BO2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BP2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BQ2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BR2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BS2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BT2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BU2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BV2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BW2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BX2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BY2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="BZ2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CA2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CB2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CC2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CD2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CE2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CF2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CG2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CH2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CI2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CJ2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CK2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CL2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CM2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CN2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CO2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CP2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CQ2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CR2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CS2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CT2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CU2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CV2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CW2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="CX2" s="26" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
@@ -3324,11 +3689,65 @@
       <c r="AT3" s="38"/>
       <c r="AU3" s="38"/>
       <c r="AV3" s="38"/>
+      <c r="AW3" s="38"/>
+      <c r="AX3" s="38"/>
+      <c r="AY3" s="38"/>
+      <c r="AZ3" s="38"/>
+      <c r="BA3" s="38"/>
+      <c r="BB3" s="38"/>
+      <c r="BC3" s="38"/>
+      <c r="BD3" s="38"/>
+      <c r="BE3" s="38"/>
+      <c r="BF3" s="38"/>
+      <c r="BG3" s="38"/>
+      <c r="BH3" s="38"/>
+      <c r="BI3" s="38"/>
+      <c r="BJ3" s="38"/>
+      <c r="BK3" s="38"/>
+      <c r="BL3" s="38"/>
+      <c r="BM3" s="38"/>
+      <c r="BN3" s="38"/>
+      <c r="BO3" s="38"/>
+      <c r="BP3" s="38"/>
+      <c r="BQ3" s="38"/>
+      <c r="BR3" s="38"/>
+      <c r="BS3" s="38"/>
+      <c r="BT3" s="38"/>
+      <c r="BU3" s="38"/>
+      <c r="BV3" s="38"/>
+      <c r="BW3" s="38"/>
+      <c r="BX3" s="38"/>
+      <c r="BY3" s="38"/>
+      <c r="BZ3" s="38"/>
+      <c r="CA3" s="38"/>
+      <c r="CB3" s="38"/>
+      <c r="CC3" s="38"/>
+      <c r="CD3" s="38"/>
+      <c r="CE3" s="38"/>
+      <c r="CF3" s="38"/>
+      <c r="CG3" s="38"/>
+      <c r="CH3" s="38"/>
+      <c r="CI3" s="38"/>
+      <c r="CJ3" s="38"/>
+      <c r="CK3" s="38"/>
+      <c r="CL3" s="38"/>
+      <c r="CM3" s="38"/>
+      <c r="CN3" s="38"/>
+      <c r="CO3" s="38"/>
+      <c r="CP3" s="38"/>
+      <c r="CQ3" s="38"/>
+      <c r="CR3" s="38"/>
+      <c r="CS3" s="38"/>
+      <c r="CT3" s="38"/>
+      <c r="CU3" s="38"/>
+      <c r="CV3" s="38"/>
+      <c r="CW3" s="38"/>
+      <c r="CX3" s="38"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -3337,22 +3756,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="3" style="0" width="16.07"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5295,7 +5713,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>